<commit_message>
Another update on 2021/02/01.
</commit_message>
<xml_diff>
--- a/python_work/currency_data.xlsx
+++ b/python_work/currency_data.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4441"/>
+  <dimension ref="A1:C4442"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49291,10 +49291,21 @@
         <v>44224</v>
       </c>
       <c r="B4441" t="n">
-        <v>15.05813026428223</v>
+        <v>15.26220035552979</v>
       </c>
       <c r="C4441" t="n">
-        <v>1.373966097831726</v>
+        <v>1.366941928863525</v>
+      </c>
+    </row>
+    <row r="4442">
+      <c r="A4442" s="2" t="n">
+        <v>44225</v>
+      </c>
+      <c r="B4442" t="n">
+        <v>15.18850040435791</v>
+      </c>
+      <c r="C4442" t="n">
+        <v>1.372500896453857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>